<commit_message>
rscript to process data
</commit_message>
<xml_diff>
--- a/treemap/CountryCodeToNameLookup.xlsx
+++ b/treemap/CountryCodeToNameLookup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lauh/Documents/GitHub/new-trade-map/treemap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{274EE342-0E71-E34C-9F76-6594EDC2F3DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F094BD-BD00-1F45-A672-17CC560C3774}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{63BEA634-3D8B-C84D-97E2-08C05778C63C}"/>
   </bookViews>
@@ -1335,9 +1335,6 @@
     <t>UM</t>
   </si>
   <si>
-    <t>United States inc Puerto Rico</t>
-  </si>
-  <si>
     <t>US</t>
   </si>
   <si>
@@ -1441,6 +1438,9 @@
   </si>
   <si>
     <t>W1</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
 </sst>
 </file>
@@ -1794,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDC35F7-5471-E64B-A9DF-6479A1C64D40}">
   <dimension ref="A1:B236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="B220" sqref="B220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3546,146 +3546,146 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B219" t="s">
-        <v>436</v>
+        <v>471</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B220" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B221" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B222" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B223" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B224" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B225" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B226" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B227" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B228" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B229" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B230" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B231" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B232" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B233" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B234" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B235" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B236" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>